<commit_message>
wrote most of final report
</commit_message>
<xml_diff>
--- a/Documentation/Other/PLED Gantt.xlsx
+++ b/Documentation/Other/PLED Gantt.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="3150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="3150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Start date</t>
   </si>
@@ -65,9 +66,6 @@
     <t>Configure communications from microcontroller to motor driver (Zach)</t>
   </si>
   <si>
-    <t>Critical Design Review (Team)</t>
-  </si>
-  <si>
     <t>Testing and Verification (Team)</t>
   </si>
   <si>
@@ -77,28 +75,16 @@
     <t>Design poster (Zach &amp; Casey)</t>
   </si>
   <si>
-    <t>CDR Slides (Zach &amp; Casey)</t>
-  </si>
-  <si>
     <t>Configure serial communications PC / microcontroller (Zach &amp; Justin)</t>
   </si>
   <si>
     <t>Test components individually (Team)</t>
   </si>
   <si>
-    <t>Write software to ingest and process image (Casey)</t>
-  </si>
-  <si>
     <t>Impliment and calibrate laser control system (Zach)</t>
   </si>
   <si>
-    <t>Mathematically Model System (Tate, Zach, Casey)</t>
-  </si>
-  <si>
     <t>Design and impliment feedback system (Tate, Zach, Casey)</t>
-  </si>
-  <si>
-    <t>Find method to convert image to G-Codes (Justin &amp; Casey)</t>
   </si>
   <si>
     <t>Write Final Report (Zach &amp; Casey)</t>
@@ -118,14 +104,48 @@
   <si>
     <t>Machine Parts (Tate)</t>
   </si>
+  <si>
+    <t>Write software to ingest and process image and convert to g-codes(Casey)</t>
+  </si>
+  <si>
+    <t>Mathematically model system (Tate, Zach, Casey)</t>
+  </si>
+  <si>
+    <t>PLED Schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Phase 1 - Initial documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Phase 2 - Build prototype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Phase 3 - Testing, final documentation, additional features</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -140,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -148,14 +168,337 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,9 +576,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:f>Sheet1!$B$2:$B$25</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>Specifications Document (Zach &amp; Casey)</c:v>
                 </c:pt>
@@ -249,16 +592,16 @@
                   <c:v>Preliminary Design Review Slides (Zach &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Preliminary Design Review (Team)</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Procure components (Zach &amp; Casey)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Preliminary Design Review (Team)</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Configure serial communications PC / microcontroller (Zach &amp; Justin)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Write software to ingest and process image (Casey)</c:v>
+                  <c:v>Write software to ingest and process image and convert to g-codes(Casey)</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Test components individually (Team)</c:v>
@@ -267,54 +610,45 @@
                   <c:v>Configure communications from microcontroller to motor driver (Zach)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Find method to convert image to G-Codes (Justin &amp; Casey)</c:v>
+                  <c:v>Design mechanical system (Tate)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Design mechanical system (Tate)</c:v>
+                  <c:v>Impliment parser for g-code files (Justin)</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Impliment parser for g-code files (Justin)</c:v>
+                  <c:v>Write software GUI and interface (Casey)</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Write software GUI and interface (Casey)</c:v>
+                  <c:v>Procure mechanical system components (Tate &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>CDR Slides (Zach &amp; Casey)</c:v>
+                  <c:v>Design and impliment feedback system (Tate, Zach, Casey)</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Procure mechanical system components (Tate &amp; Casey)</c:v>
+                  <c:v>Mathematically model system (Tate, Zach, Casey)</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Design and impliment feedback system (Tate, Zach, Casey)</c:v>
+                  <c:v>Impliment and calibrate laser control system (Zach)</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Critical Design Review (Team)</c:v>
+                  <c:v>Integrate G-Code interpreter into microcontroller (Justin)</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Mathematically Model System (Tate, Zach, Casey)</c:v>
+                  <c:v>Machine Parts (Tate)</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Impliment and calibrate laser control system (Zach)</c:v>
+                  <c:v>Assemble system (Team)</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Integrate G-Code interpreter into microcontroller (Justin)</c:v>
+                  <c:v>Write User's Manual (Zach &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Machine Parts (Tate)</c:v>
+                  <c:v>Write Final Report (Zach &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Assemble system (Team)</c:v>
+                  <c:v>Testing and Verification (Team)</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Testing and Verification (Team)</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Write User's Manual (Zach &amp; Casey)</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Write Final Report (Zach &amp; Casey)</c:v>
-                </c:pt>
-                <c:pt idx="26">
                   <c:v>Design poster (Zach &amp; Casey)</c:v>
                 </c:pt>
               </c:strCache>
@@ -322,10 +656,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$28</c:f>
+              <c:f>Sheet1!$C$2:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>42339</c:v>
                 </c:pt>
@@ -339,10 +673,10 @@
                   <c:v>42370</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>42396</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>42370</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42396</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>42384</c:v>
@@ -357,54 +691,45 @@
                   <c:v>42409</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42409</c:v>
+                  <c:v>42389</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42389</c:v>
+                  <c:v>42420</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>42421</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42433</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42434</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>42420</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>42421</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>42430</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42433</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42434</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42444</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42420</c:v>
+                  <c:v>42444</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42421</c:v>
+                  <c:v>42461</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42444</c:v>
+                  <c:v>42461</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42444</c:v>
+                  <c:v>42461</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42461</c:v>
+                  <c:v>42468</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42468</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>42461</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>42461</c:v>
-                </c:pt>
-                <c:pt idx="26">
                   <c:v>42475</c:v>
                 </c:pt>
               </c:numCache>
@@ -443,9 +768,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -461,9 +784,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -482,7 +803,6 @@
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                  <a:alpha val="30000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="0">
@@ -499,9 +819,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -517,8 +835,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="30000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="0">
@@ -535,11 +854,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -555,9 +870,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7030A0">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -573,9 +886,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B050">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -594,7 +905,6 @@
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                  <a:alpha val="30000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="0">
@@ -611,9 +921,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -629,10 +937,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -648,9 +953,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -666,9 +969,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -684,9 +985,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B050">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -702,15 +1001,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="30000"/>
-                </a:schemeClr>
+                <a:srgbClr val="002060"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:alpha val="30000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="bg1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -722,9 +1017,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="92D050">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:srgbClr val="002060"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -740,9 +1033,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="002060">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -758,10 +1049,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="30000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="0">
@@ -778,9 +1067,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="002060">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -796,9 +1083,10 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -814,10 +1102,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                  <a:alpha val="65000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -833,7 +1118,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -868,64 +1153,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="24"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="90000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="25"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="90000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="26"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="90000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="0">
                 <a:solidFill>
@@ -937,9 +1165,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:f>Sheet1!$B$2:$B$25</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>Specifications Document (Zach &amp; Casey)</c:v>
                 </c:pt>
@@ -953,16 +1181,16 @@
                   <c:v>Preliminary Design Review Slides (Zach &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Preliminary Design Review (Team)</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Procure components (Zach &amp; Casey)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Preliminary Design Review (Team)</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Configure serial communications PC / microcontroller (Zach &amp; Justin)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Write software to ingest and process image (Casey)</c:v>
+                  <c:v>Write software to ingest and process image and convert to g-codes(Casey)</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Test components individually (Team)</c:v>
@@ -971,54 +1199,45 @@
                   <c:v>Configure communications from microcontroller to motor driver (Zach)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Find method to convert image to G-Codes (Justin &amp; Casey)</c:v>
+                  <c:v>Design mechanical system (Tate)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Design mechanical system (Tate)</c:v>
+                  <c:v>Impliment parser for g-code files (Justin)</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Impliment parser for g-code files (Justin)</c:v>
+                  <c:v>Write software GUI and interface (Casey)</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Write software GUI and interface (Casey)</c:v>
+                  <c:v>Procure mechanical system components (Tate &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>CDR Slides (Zach &amp; Casey)</c:v>
+                  <c:v>Design and impliment feedback system (Tate, Zach, Casey)</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Procure mechanical system components (Tate &amp; Casey)</c:v>
+                  <c:v>Mathematically model system (Tate, Zach, Casey)</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Design and impliment feedback system (Tate, Zach, Casey)</c:v>
+                  <c:v>Impliment and calibrate laser control system (Zach)</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Critical Design Review (Team)</c:v>
+                  <c:v>Integrate G-Code interpreter into microcontroller (Justin)</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Mathematically Model System (Tate, Zach, Casey)</c:v>
+                  <c:v>Machine Parts (Tate)</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Impliment and calibrate laser control system (Zach)</c:v>
+                  <c:v>Assemble system (Team)</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Integrate G-Code interpreter into microcontroller (Justin)</c:v>
+                  <c:v>Write User's Manual (Zach &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Machine Parts (Tate)</c:v>
+                  <c:v>Write Final Report (Zach &amp; Casey)</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Assemble system (Team)</c:v>
+                  <c:v>Testing and Verification (Team)</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Testing and Verification (Team)</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Write User's Manual (Zach &amp; Casey)</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Write Final Report (Zach &amp; Casey)</c:v>
-                </c:pt>
-                <c:pt idx="26">
                   <c:v>Design poster (Zach &amp; Casey)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1026,10 +1245,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$28</c:f>
+              <c:f>Sheet1!$E$2:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>14</c:v>
                 </c:pt>
@@ -1043,10 +1262,10 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>24</c:v>
@@ -1061,54 +1280,45 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>23</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>34</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="26">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -1125,11 +1335,11 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="207343760"/>
-        <c:axId val="207346504"/>
+        <c:axId val="291139072"/>
+        <c:axId val="291142600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="207343760"/>
+        <c:axId val="291139072"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1172,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207346504"/>
+        <c:crossAx val="291142600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1180,7 +1390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="207346504"/>
+        <c:axId val="291142600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42495"/>
@@ -1233,7 +1443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207343760"/>
+        <c:crossAx val="291139072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1834,13 +2044,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>381679</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>121099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>356187</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>151039</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2126,10 +2336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E28"/>
+  <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E28" sqref="B1:E28"/>
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E25" sqref="B1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,7 +2376,7 @@
         <v>42353</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E28" si="0">(D2-C2)</f>
+        <f>(D2-C2)</f>
         <v>14</v>
       </c>
     </row>
@@ -2181,7 +2391,7 @@
         <v>42353</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" si="0"/>
+        <f>(D3-C3)</f>
         <v>14</v>
       </c>
     </row>
@@ -2196,7 +2406,7 @@
         <v>42394</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
+        <f>(D4-C4)</f>
         <v>41</v>
       </c>
     </row>
@@ -2211,43 +2421,43 @@
         <v>42394</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f>(D5-C5)</f>
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>42370</v>
+        <v>42396</v>
       </c>
       <c r="D6" s="1">
-        <v>42394</v>
+        <v>42397</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f>(D6-C6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>42396</v>
+        <v>42370</v>
       </c>
       <c r="D7" s="1">
-        <v>42397</v>
+        <v>42399</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>(D7-C7)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>42384</v>
@@ -2256,13 +2466,13 @@
         <v>42408</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f>(D8-C8)</f>
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1">
         <v>42394</v>
@@ -2271,13 +2481,13 @@
         <v>42408</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f>(D9-C9)</f>
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
         <v>42384</v>
@@ -2286,7 +2496,7 @@
         <v>42410</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
+        <f>(D10-C10)</f>
         <v>26</v>
       </c>
     </row>
@@ -2301,83 +2511,83 @@
         <v>42420</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f>(D11-C11)</f>
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>42409</v>
+        <v>42389</v>
       </c>
       <c r="D12" s="1">
-        <v>42420</v>
+        <v>42429</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>(D12-C12)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1">
-        <v>42389</v>
+        <v>42420</v>
       </c>
       <c r="D13" s="1">
-        <v>42429</v>
+        <v>42444</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>(D13-C13)</f>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
-        <v>42420</v>
+        <v>42421</v>
       </c>
       <c r="D14" s="1">
         <v>42444</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f>(D14-C14)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1">
-        <v>42421</v>
+        <v>42433</v>
       </c>
       <c r="D15" s="1">
         <v>42444</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f>(D15-C15)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
-        <v>42430</v>
+        <v>42434</v>
       </c>
       <c r="D16" s="1">
         <v>42444</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f>(D16-C16)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -2385,59 +2595,59 @@
         <v>27</v>
       </c>
       <c r="C17" s="1">
-        <v>42433</v>
+        <v>42420</v>
       </c>
       <c r="D17" s="1">
-        <v>42444</v>
+        <v>42454</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>(D17-C17)</f>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1">
-        <v>42434</v>
+        <v>42421</v>
       </c>
       <c r="D18" s="1">
-        <v>42444</v>
+        <v>42454</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>(D18-C18)</f>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1">
         <v>42444</v>
       </c>
       <c r="D19" s="1">
-        <v>42445</v>
+        <v>42454</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>(D19-C19)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1">
-        <v>42420</v>
+        <v>42444</v>
       </c>
       <c r="D20" s="1">
-        <v>42454</v>
+        <v>42460</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <f>(D20-C20)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -2445,128 +2655,517 @@
         <v>21</v>
       </c>
       <c r="C21" s="1">
-        <v>42421</v>
+        <v>42461</v>
       </c>
       <c r="D21" s="1">
-        <v>42454</v>
+        <v>42468</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <f>(D21-C21)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>42444</v>
+        <v>42461</v>
       </c>
       <c r="D22" s="1">
-        <v>42454</v>
+        <v>42489</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>(D22-C22)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1">
-        <v>42444</v>
+        <v>42461</v>
       </c>
       <c r="D23" s="1">
-        <v>42460</v>
+        <v>42489</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>(D23-C23)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1">
-        <v>42461</v>
+        <v>42468</v>
       </c>
       <c r="D24" s="1">
-        <v>42468</v>
+        <v>42489</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>(D24-C24)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
-        <v>42468</v>
+        <v>42475</v>
       </c>
       <c r="D25" s="1">
         <v>42489</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="1">
-        <v>42461</v>
-      </c>
-      <c r="D26" s="1">
-        <v>42489</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="1">
-        <v>42461</v>
-      </c>
-      <c r="D27" s="1">
-        <v>42489</v>
-      </c>
-      <c r="E27" s="2">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="1">
-        <v>42475</v>
-      </c>
-      <c r="D28" s="1">
-        <v>42489</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" si="0"/>
+        <f>(D25-C25)</f>
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:E27">
-    <sortCondition ref="D2:D27"/>
-    <sortCondition ref="C2:C27"/>
+  <sortState ref="B2:E25">
+    <sortCondition ref="D2:D25"/>
+    <sortCondition ref="C2:C25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="B2:E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10">
+        <v>42339</v>
+      </c>
+      <c r="D5" s="9">
+        <v>42353</v>
+      </c>
+      <c r="E5" s="18">
+        <f>(D5-C5)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>42339</v>
+      </c>
+      <c r="D6" s="11">
+        <v>42353</v>
+      </c>
+      <c r="E6" s="19">
+        <f>(D6-C6)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12">
+        <v>42353</v>
+      </c>
+      <c r="D7" s="11">
+        <v>42394</v>
+      </c>
+      <c r="E7" s="19">
+        <f>(D7-C7)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="12">
+        <v>42370</v>
+      </c>
+      <c r="D8" s="11">
+        <v>42394</v>
+      </c>
+      <c r="E8" s="19">
+        <f>(D8-C8)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="14">
+        <v>42396</v>
+      </c>
+      <c r="D9" s="13">
+        <v>42397</v>
+      </c>
+      <c r="E9" s="20">
+        <f>(D9-C9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9">
+        <v>42370</v>
+      </c>
+      <c r="D11" s="10">
+        <v>42399</v>
+      </c>
+      <c r="E11" s="15">
+        <f>(D11-C11)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="11">
+        <v>42384</v>
+      </c>
+      <c r="D12" s="12">
+        <v>42408</v>
+      </c>
+      <c r="E12" s="16">
+        <f>(D12-C12)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="11">
+        <v>42394</v>
+      </c>
+      <c r="D13" s="12">
+        <v>42408</v>
+      </c>
+      <c r="E13" s="16">
+        <f>(D13-C13)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="11">
+        <v>42384</v>
+      </c>
+      <c r="D14" s="12">
+        <v>42410</v>
+      </c>
+      <c r="E14" s="16">
+        <f>(D14-C14)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="11">
+        <v>42409</v>
+      </c>
+      <c r="D15" s="12">
+        <v>42420</v>
+      </c>
+      <c r="E15" s="16">
+        <f>(D15-C15)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="11">
+        <v>42389</v>
+      </c>
+      <c r="D16" s="12">
+        <v>42429</v>
+      </c>
+      <c r="E16" s="16">
+        <f>(D16-C16)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="11">
+        <v>42420</v>
+      </c>
+      <c r="D17" s="12">
+        <v>42444</v>
+      </c>
+      <c r="E17" s="16">
+        <f>(D17-C17)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="11">
+        <v>42421</v>
+      </c>
+      <c r="D18" s="12">
+        <v>42444</v>
+      </c>
+      <c r="E18" s="16">
+        <f>(D18-C18)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="11">
+        <v>42433</v>
+      </c>
+      <c r="D19" s="12">
+        <v>42444</v>
+      </c>
+      <c r="E19" s="16">
+        <f>(D19-C19)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="11">
+        <v>42434</v>
+      </c>
+      <c r="D20" s="12">
+        <v>42444</v>
+      </c>
+      <c r="E20" s="16">
+        <f>(D20-C20)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="11">
+        <v>42420</v>
+      </c>
+      <c r="D21" s="12">
+        <v>42454</v>
+      </c>
+      <c r="E21" s="16">
+        <f>(D21-C21)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="11">
+        <v>42421</v>
+      </c>
+      <c r="D22" s="12">
+        <v>42454</v>
+      </c>
+      <c r="E22" s="16">
+        <f>(D22-C22)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="11">
+        <v>42444</v>
+      </c>
+      <c r="D23" s="12">
+        <v>42454</v>
+      </c>
+      <c r="E23" s="16">
+        <f>(D23-C23)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="11">
+        <v>42444</v>
+      </c>
+      <c r="D24" s="12">
+        <v>42460</v>
+      </c>
+      <c r="E24" s="16">
+        <f>(D24-C24)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="13">
+        <v>42461</v>
+      </c>
+      <c r="D25" s="14">
+        <v>42468</v>
+      </c>
+      <c r="E25" s="17">
+        <f>(D25-C25)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="9">
+        <v>42461</v>
+      </c>
+      <c r="D27" s="10">
+        <v>42489</v>
+      </c>
+      <c r="E27" s="15">
+        <f>(D27-C27)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="11">
+        <v>42461</v>
+      </c>
+      <c r="D28" s="12">
+        <v>42489</v>
+      </c>
+      <c r="E28" s="16">
+        <f>(D28-C28)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="11">
+        <v>42468</v>
+      </c>
+      <c r="D29" s="12">
+        <v>42489</v>
+      </c>
+      <c r="E29" s="16">
+        <f>(D29-C29)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="13">
+        <v>42475</v>
+      </c>
+      <c r="D30" s="14">
+        <v>42489</v>
+      </c>
+      <c r="E30" s="17">
+        <f>(D30-C30)</f>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B26:E26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>